<commit_message>
📊 Arribos 141 actualizados - 18
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,16 +465,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>15:50</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -485,16 +485,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -505,16 +505,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -525,16 +525,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -545,16 +545,16 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>15:40</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -565,16 +565,16 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>16:02</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -585,36 +585,36 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>16:04</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>16:08</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -625,56 +625,56 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>16:13</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -685,16 +685,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>16:02</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -705,16 +705,16 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>16:04</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -725,16 +725,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>16:13</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -745,36 +745,36 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16:19</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -785,36 +785,36 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:43</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>16:29</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -825,16 +825,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -845,16 +845,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -865,36 +865,36 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>16:39</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -905,36 +905,36 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>17:06</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -945,16 +945,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -985,16 +985,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1005,60 +1005,40 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>17:24</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>108</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
@@ -1073,7 +1053,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1112,36 +1092,36 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>16:13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>15:40</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1152,16 +1132,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>16:13</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1172,16 +1152,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>16:19</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1192,16 +1172,16 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1212,38 +1192,18 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="D7" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>17:14</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>98</v>
-      </c>
-      <c r="D8" t="inlineStr">
         <is>
           <t>📅</t>
         </is>
@@ -1260,7 +1220,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1299,16 +1259,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>15:50</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -1319,16 +1279,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>15:53</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1339,16 +1299,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>15:37</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1359,16 +1319,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>15:38</t>
+          <t>15:56</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1379,16 +1339,16 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>15:40</t>
+          <t>16:01</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1399,16 +1359,16 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>16:02</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -1419,36 +1379,36 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>15:46</t>
+          <t>16:04</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>16:08</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1459,56 +1419,56 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>16:13</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1519,16 +1479,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>16:02</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1539,16 +1499,16 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>16:04</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1559,16 +1519,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>16:13</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1579,36 +1539,36 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16:19</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1619,36 +1579,36 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:43</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>16:29</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1659,16 +1619,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1679,16 +1639,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1699,36 +1659,36 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>16:39</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1739,36 +1699,36 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>17:06</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1779,16 +1739,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1799,16 +1759,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1819,16 +1779,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1839,60 +1799,40 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>17:24</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>108</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 19
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,16 +465,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>15:50</t>
+          <t>15:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -485,16 +485,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:51</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -505,20 +505,20 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:55</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
@@ -530,15 +530,15 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -554,7 +554,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -574,7 +574,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -594,7 +594,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -614,7 +614,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -634,7 +634,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -654,7 +654,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -665,7 +665,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:19</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -674,7 +674,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -694,7 +694,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -714,7 +714,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -734,7 +734,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -774,7 +774,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -794,7 +794,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -814,7 +814,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -825,12 +825,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>16:52</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -845,16 +845,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -865,16 +865,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -885,16 +885,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -905,16 +905,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>17:06</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -925,16 +925,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -945,16 +945,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1014,7 +1014,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1034,9 +1034,29 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D30" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>119</v>
+      </c>
+      <c r="D31" t="inlineStr">
         <is>
           <t>📅</t>
         </is>
@@ -1101,7 +1121,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -1112,7 +1132,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:19</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1121,7 +1141,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1132,7 +1152,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:52</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1141,7 +1161,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1161,7 +1181,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1181,7 +1201,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1201,7 +1221,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -1220,7 +1240,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1259,16 +1279,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>15:50</t>
+          <t>15:51</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -1279,16 +1299,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>15:53</t>
+          <t>15:51</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1299,20 +1319,20 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>15:55</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
@@ -1324,15 +1344,15 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -1348,7 +1368,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1368,7 +1388,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -1388,7 +1408,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1408,7 +1428,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1428,7 +1448,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1448,7 +1468,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1459,7 +1479,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:19</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1468,7 +1488,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1488,7 +1508,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1508,7 +1528,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1528,7 +1548,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1548,7 +1568,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1568,7 +1588,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1588,7 +1608,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1608,7 +1628,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1619,12 +1639,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>16:52</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -1639,16 +1659,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1659,16 +1679,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1679,16 +1699,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:07</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1699,16 +1719,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>17:06</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1719,16 +1739,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1739,16 +1759,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:24</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1759,16 +1779,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1788,7 +1808,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1808,7 +1828,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1828,9 +1848,29 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D30" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>17:50</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>119</v>
+      </c>
+      <c r="D31" t="inlineStr">
         <is>
           <t>📅</t>
         </is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 20
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,12 +465,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>15:51</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -478,14 +478,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>15:51</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -505,36 +505,36 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>16:17</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -545,56 +545,56 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:02</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:04</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -605,16 +605,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>16:08</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -625,12 +625,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>16:13</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -645,16 +645,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -665,12 +665,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>16:19</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -685,36 +685,36 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:43</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>16:29</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -725,16 +725,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -745,16 +745,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -765,16 +765,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -785,36 +785,36 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -825,16 +825,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -845,16 +845,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -865,16 +865,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -885,16 +885,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -905,16 +905,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -925,27 +925,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:41</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -954,7 +954,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:43</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -985,16 +985,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1005,58 +1005,78 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D31" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>110</v>
+      </c>
+      <c r="D32" t="inlineStr">
         <is>
           <t>📅</t>
         </is>
@@ -1073,7 +1093,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1112,7 +1132,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16:13</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1121,18 +1141,18 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>22</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>16:19</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1141,18 +1161,18 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1161,7 +1181,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1181,7 +1201,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1201,7 +1221,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1221,9 +1241,29 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="D7" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>110</v>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>📅</t>
         </is>
@@ -1240,7 +1280,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1279,12 +1319,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>15:51</t>
+          <t>16:14</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1292,14 +1332,14 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>15:51</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1308,7 +1348,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1319,36 +1359,36 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>15:55</t>
+          <t>16:15</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>15:56</t>
+          <t>16:17</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>225_C ROCA-H SUR</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1359,56 +1399,56 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:01</t>
+          <t>16:20</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:02</t>
+          <t>16:21</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:04</t>
+          <t>16:29</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1419,16 +1459,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>16:08</t>
+          <t>16:30</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1439,12 +1479,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>16:13</t>
+          <t>16:36</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -1459,16 +1499,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>16:40</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1479,12 +1519,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>16:19</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -1499,36 +1539,36 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:43</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>16:29</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1539,16 +1579,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1559,16 +1599,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:53</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1579,16 +1619,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1599,36 +1639,36 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1639,16 +1679,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1659,16 +1699,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1679,16 +1719,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1699,16 +1739,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>17:07</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1719,16 +1759,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1739,27 +1779,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>17:24</t>
+          <t>17:41</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1768,7 +1808,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1779,16 +1819,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:43</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1799,16 +1839,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:44</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1819,58 +1859,78 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="D31" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>18:04</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>110</v>
+      </c>
+      <c r="D32" t="inlineStr">
         <is>
           <t>📅</t>
         </is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 21
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,27 +465,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>16:35</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>16:35</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -505,36 +505,36 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>16:39</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>16:17</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -545,16 +545,16 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -565,36 +565,36 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:29</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -605,16 +605,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:51</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -625,16 +625,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:52</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -645,36 +645,36 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -685,56 +685,56 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -745,16 +745,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -765,16 +765,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>17:13</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -785,16 +785,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -805,16 +805,16 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -825,16 +825,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -845,16 +845,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -865,16 +865,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:37</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -885,36 +885,36 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -925,16 +925,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -945,7 +945,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>17:41</t>
+          <t>18:02</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -954,7 +954,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,12 +965,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>17:43</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -985,12 +985,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1005,36 +1005,36 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1045,40 +1045,20 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
           <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>18:04</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>110</v>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>📅</t>
         </is>
       </c>
     </row>
@@ -1093,7 +1073,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1132,36 +1112,36 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>16:52</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1172,12 +1152,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>17:13</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -1192,36 +1172,36 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>60</v>
+        <v>89</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1232,40 +1212,20 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>86</v>
+        <v>113</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>📅</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>18:04</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>110</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -1280,7 +1240,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1319,27 +1279,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16:14</t>
+          <t>16:35</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>16:35</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1359,36 +1319,36 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>16:15</t>
+          <t>16:39</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>16:17</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>225_C ROCA-H SUR</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1399,16 +1359,16 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:20</t>
+          <t>16:42</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1419,36 +1379,36 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:21</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:29</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1459,16 +1419,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>16:30</t>
+          <t>16:51</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1479,16 +1439,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>16:36</t>
+          <t>16:52</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1499,36 +1459,36 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>16:40</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1539,56 +1499,56 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>16:43</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1599,16 +1559,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>16:53</t>
+          <t>17:09</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1619,16 +1579,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>17:13</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1639,16 +1599,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1659,16 +1619,16 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1679,16 +1639,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1699,16 +1659,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1719,16 +1679,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:37</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1739,36 +1699,36 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:39</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1779,16 +1739,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1799,7 +1759,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>17:41</t>
+          <t>18:02</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1808,7 +1768,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1819,12 +1779,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>17:43</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1839,12 +1799,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>17:44</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1859,36 +1819,36 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>98</v>
+        <v>113</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1899,40 +1859,20 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
           <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>18:04</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="C32" t="n">
-        <v>110</v>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>📅</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 22
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,7 +465,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16:35</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -474,7 +474,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -485,16 +485,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>16:35</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -505,36 +505,36 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>16:39</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:49</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -545,36 +545,36 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:55</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -585,16 +585,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -605,16 +605,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>16:51</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -625,16 +625,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -645,16 +645,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -665,12 +665,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -685,16 +685,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -705,36 +705,36 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -745,16 +745,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>17:09</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -765,16 +765,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>17:13</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -785,16 +785,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -805,47 +805,47 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -854,7 +854,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -865,16 +865,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>17:37</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -885,16 +885,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -905,16 +905,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -925,27 +925,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>18:02</t>
+          <t>18:14</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -954,7 +954,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -985,16 +985,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1005,58 +1005,18 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>18:20</t>
+          <t>18:32</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D29" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>18:27</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>113</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>18:31</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>11X44_ETCHEVERRY</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>117</v>
-      </c>
-      <c r="D31" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -1112,7 +1072,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>16:49</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1121,7 +1081,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -1141,18 +1101,18 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>17:13</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1161,7 +1121,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1172,7 +1132,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1181,7 +1141,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1201,7 +1161,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1221,7 +1181,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -1240,7 +1200,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1279,7 +1239,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16:35</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1288,7 +1248,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -1299,16 +1259,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>16:35</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1319,36 +1279,36 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>16:39</t>
+          <t>16:48</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:49</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1359,36 +1319,36 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:42</t>
+          <t>16:55</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>16:56</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>17_179 Y 38</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -1399,16 +1359,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:50</t>
+          <t>16:57</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1419,16 +1379,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>16:51</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1439,16 +1399,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>16:52</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1459,16 +1419,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>17:04</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1479,12 +1439,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>17:10</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -1499,16 +1459,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:14</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1519,36 +1479,36 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1559,16 +1519,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>17:09</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1579,16 +1539,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>17:13</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1599,16 +1559,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1619,47 +1579,47 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -1668,7 +1628,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1679,16 +1639,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>17:37</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1699,16 +1659,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>17:39</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1719,16 +1679,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1739,27 +1699,27 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>18:02</t>
+          <t>18:14</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1768,7 +1728,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1779,16 +1739,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1799,16 +1759,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1819,58 +1779,18 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>18:20</t>
+          <t>18:32</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D29" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>18:27</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>215C_EL PATO</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>113</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>18:31</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>11X44_ETCHEVERRY</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>117</v>
-      </c>
-      <c r="D31" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 23
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,7 +465,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>17:12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -485,16 +485,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>17:13</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -505,16 +505,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -525,16 +525,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>16:49</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -545,36 +545,36 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:55</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -585,16 +585,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -605,16 +605,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -625,16 +625,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -645,16 +645,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -665,36 +665,36 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -705,12 +705,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -718,19 +718,19 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -745,16 +745,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -765,36 +765,36 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -805,7 +805,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -814,7 +814,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -825,36 +825,36 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>18:08</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>18:12</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -865,16 +865,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -885,36 +885,36 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -925,16 +925,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:39</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -945,16 +945,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>18:14</t>
+          <t>18:47</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -985,40 +985,80 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>19:03</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>112</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>19:10</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>118</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>📅</t>
         </is>
       </c>
     </row>
@@ -1033,7 +1073,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1072,12 +1112,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16:49</t>
+          <t>17:13</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1092,36 +1132,36 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1132,36 +1172,36 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>75</v>
+        <v>99</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1172,20 +1212,40 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>19:03</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>111</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>📅</t>
         </is>
       </c>
     </row>
@@ -1200,7 +1260,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1239,7 +1299,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>17:12</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1259,16 +1319,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>17:13</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1279,16 +1339,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>16:48</t>
+          <t>17:16</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1299,16 +1359,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>16:49</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1319,36 +1379,36 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>16:55</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>16:56</t>
+          <t>17:21</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>17_179 Y 38</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -1359,16 +1419,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>16:57</t>
+          <t>17:28</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1379,16 +1439,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:33</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1399,16 +1459,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:34</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1419,16 +1479,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>17:04</t>
+          <t>17:36</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1439,36 +1499,36 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>17:10</t>
+          <t>17:38</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>17:14</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1479,12 +1539,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:40</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -1492,19 +1552,19 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -1519,16 +1579,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>17:50</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1539,36 +1599,36 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>18:03</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1579,7 +1639,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -1588,7 +1648,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1599,36 +1659,36 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>18:08</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>18:12</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1639,16 +1699,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1659,36 +1719,36 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1699,16 +1759,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:39</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1719,16 +1779,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>18:14</t>
+          <t>18:47</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1739,16 +1799,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1759,40 +1819,80 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>19:03</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>19:04</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>112</v>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>19:10</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>118</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>📅</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 24
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,12 +465,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>17:12</t>
+          <t>17:42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -485,16 +485,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>17:13</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -505,16 +505,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -525,36 +525,36 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -565,16 +565,16 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>18:01</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -585,16 +585,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -605,16 +605,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -625,7 +625,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -634,7 +634,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -645,16 +645,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>18:09</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -665,36 +665,36 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>18:11</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -705,36 +705,36 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -745,16 +745,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -765,36 +765,36 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>18:28</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:32</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -805,36 +805,36 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>18:08</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -845,16 +845,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>18:12</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -865,16 +865,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>18:20</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -885,76 +885,76 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>18:39</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>18:47</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>18:51</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -985,16 +985,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1005,60 +1005,20 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:03</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>📅</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>19:04</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>11_ETCHEVERRY</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>112</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>19:10</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>16_P MOR-SANTA ANA</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>118</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -1073,7 +1033,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1112,16 +1072,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>17:13</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>22</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -1132,36 +1092,36 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>18:28</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1172,80 +1132,60 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18:51</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>📅</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>19:03</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>111</v>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -1260,7 +1200,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1299,12 +1239,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>17:12</t>
+          <t>17:42</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -1319,16 +1259,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>17:13</t>
+          <t>17:45</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1339,16 +1279,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>17:16</t>
+          <t>17:51</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1359,36 +1299,36 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:52</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>17:53</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1399,16 +1339,16 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>17:21</t>
+          <t>18:01</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -1419,16 +1359,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>17:28</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1439,16 +1379,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>17:33</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1459,7 +1399,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>17:34</t>
+          <t>18:05</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1468,7 +1408,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1479,16 +1419,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>17:36</t>
+          <t>18:09</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1499,36 +1439,36 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>17:38</t>
+          <t>18:11</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1539,36 +1479,36 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>17:40</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1579,16 +1519,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>17:50</t>
+          <t>18:25</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1599,36 +1539,36 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>18:28</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>18:03</t>
+          <t>18:32</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1639,36 +1579,36 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>18:08</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1679,16 +1619,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>18:12</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1699,16 +1639,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>18:20</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1719,76 +1659,76 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:59</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>18:39</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>18:47</t>
+          <t>19:11</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1799,16 +1739,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>18:51</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1819,16 +1759,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1839,60 +1779,20 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:03</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>📅</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>19:04</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>11_ETCHEVERRY</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>112</v>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>19:10</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>16_P MOR-SANTA ANA</t>
-        </is>
-      </c>
-      <c r="C31" t="n">
-        <v>118</v>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 25
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,16 +465,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -485,36 +485,36 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -525,12 +525,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>18:08</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -538,43 +538,43 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18:01</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -585,16 +585,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -605,12 +605,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -625,12 +625,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -645,7 +645,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>18:09</t>
+          <t>18:24</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -654,7 +654,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -665,12 +665,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>18:11</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -685,16 +685,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -705,16 +705,16 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:34</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -725,16 +725,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -745,16 +745,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:47</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -765,16 +765,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -785,16 +785,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -805,56 +805,56 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -865,16 +865,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -885,36 +885,36 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -925,36 +925,36 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>19:47</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:49</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -985,38 +985,58 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D29" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>115</v>
+      </c>
+      <c r="D30" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -1033,7 +1053,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1072,7 +1092,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1081,7 +1101,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -1092,7 +1112,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1101,7 +1121,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1112,7 +1132,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1121,7 +1141,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1132,7 +1152,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1141,7 +1161,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1152,7 +1172,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1161,18 +1181,18 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1181,9 +1201,29 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="D7" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>115</v>
+      </c>
+      <c r="D8" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -1200,7 +1240,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1239,16 +1279,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>17:42</t>
+          <t>18:00</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -1259,36 +1299,36 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>17:45</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>17:51</t>
+          <t>18:04</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1299,12 +1339,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>17:52</t>
+          <t>18:08</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -1312,43 +1352,43 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>17:53</t>
+          <t>18:10</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18:01</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -1359,16 +1399,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:16</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1379,12 +1419,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:20</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -1399,12 +1439,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>18:05</t>
+          <t>18:21</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -1419,7 +1459,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>18:09</t>
+          <t>18:24</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1428,7 +1468,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1439,12 +1479,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>18:11</t>
+          <t>18:27</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -1459,16 +1499,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1479,16 +1519,16 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:34</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1499,16 +1539,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1519,16 +1559,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>18:25</t>
+          <t>18:47</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1539,16 +1579,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>18:28</t>
+          <t>18:51</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1559,16 +1599,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>18:32</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1579,56 +1619,56 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1639,16 +1679,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1659,36 +1699,36 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>18:59</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:29</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1699,36 +1739,36 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:39</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>83</v>
+        <v>101</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:11</t>
+          <t>19:47</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>89</v>
+        <v>109</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1739,16 +1779,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:49</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -1759,38 +1799,58 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D29" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>19:53</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>115</v>
+      </c>
+      <c r="D30" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 26
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,16 +465,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -485,27 +485,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -514,7 +514,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -525,7 +525,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18:08</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -538,23 +538,23 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -565,12 +565,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -585,16 +585,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -605,16 +605,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>18:20</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -625,36 +625,36 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -665,16 +665,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -685,16 +685,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -705,16 +705,16 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>18:34</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -725,16 +725,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -745,16 +745,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>18:47</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -765,16 +765,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>18:51</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -785,16 +785,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -805,36 +805,36 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -845,16 +845,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -865,16 +865,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -885,16 +885,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -905,36 +905,36 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -945,16 +945,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:47</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,36 +965,36 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>19:49</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1005,16 +1005,16 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1025,18 +1025,38 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>19:53</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D30" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>113</v>
+      </c>
+      <c r="D31" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -1053,7 +1073,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1092,16 +1112,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -1112,36 +1132,36 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18:51</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1152,36 +1172,36 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1192,38 +1212,18 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>20:23</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="D7" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>19:53</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>115</v>
-      </c>
-      <c r="D8" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -1240,7 +1240,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1279,16 +1279,16 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>18:00</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -1299,27 +1299,27 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18:04</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1328,7 +1328,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1339,7 +1339,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18:08</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1352,23 +1352,23 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18:10</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1379,12 +1379,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -1399,16 +1399,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>18:16</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1419,16 +1419,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>18:20</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1439,36 +1439,36 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>18:21</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>18:24</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1479,16 +1479,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>18:27</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1499,16 +1499,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1519,16 +1519,16 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>18:34</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1539,16 +1539,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1559,16 +1559,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>18:47</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1579,16 +1579,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>18:51</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1599,16 +1599,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1619,36 +1619,36 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1659,16 +1659,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1679,16 +1679,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1699,16 +1699,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1719,36 +1719,36 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:29</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>19:39</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1759,16 +1759,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:47</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>109</v>
+        <v>84</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1779,36 +1779,36 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>19:49</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1819,16 +1819,16 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1839,18 +1839,38 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>19:53</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D30" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>113</v>
+      </c>
+      <c r="D31" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 28
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -565,16 +565,16 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -585,16 +585,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -605,16 +605,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -625,36 +625,36 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -665,16 +665,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -685,36 +685,36 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -725,16 +725,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -745,16 +745,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -765,7 +765,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -774,27 +774,27 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -805,16 +805,16 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -825,16 +825,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -845,16 +845,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -865,16 +865,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -885,16 +885,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -905,16 +905,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -925,16 +925,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -945,16 +945,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,36 +965,36 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1005,16 +1005,16 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1025,40 +1025,280 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>70</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>70</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>80</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>80</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>81</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>84</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>89</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>100</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>108</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>111</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>112</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>20:23</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B42" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="C42" t="n">
         <v>113</v>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>🚌</t>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>116</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>📅</t>
         </is>
       </c>
     </row>
@@ -1073,7 +1313,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1152,7 +1392,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1161,7 +1401,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1172,16 +1412,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1192,16 +1432,16 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1212,20 +1452,60 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>84</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>20:23</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="C8" t="n">
         <v>113</v>
       </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>🚌</t>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>116</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>📅</t>
         </is>
       </c>
     </row>
@@ -1240,7 +1520,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1379,16 +1659,16 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -1399,16 +1679,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1419,16 +1699,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1439,36 +1719,36 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1479,16 +1759,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1499,36 +1779,36 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1539,16 +1819,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1559,16 +1839,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1579,7 +1859,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -1588,27 +1868,27 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -1619,16 +1899,16 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1639,16 +1919,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1659,16 +1939,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1679,16 +1959,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1699,16 +1979,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -1719,16 +1999,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1739,16 +2019,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1759,16 +2039,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1779,36 +2059,36 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1819,16 +2099,16 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1839,40 +2119,280 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>112</v>
+        <v>60</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>70</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>70</v>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>80</v>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>80</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>81</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>84</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>89</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>100</v>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>108</v>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>111</v>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>112</v>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
           <t>20:23</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B42" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="C31" t="n">
+      <c r="C42" t="n">
         <v>113</v>
       </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>🚌</t>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>116</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>📅</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 29
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,16 +485,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>18:47</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -505,16 +505,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -525,20 +525,20 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -558,23 +558,23 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -585,16 +585,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -605,16 +605,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -625,16 +625,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -645,16 +645,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -665,16 +665,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -685,56 +685,56 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -745,16 +745,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -770,7 +770,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -778,43 +778,43 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -825,20 +825,20 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -850,7 +850,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -858,23 +858,23 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -890,7 +890,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -905,16 +905,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -925,16 +925,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -945,16 +945,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -990,7 +990,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1005,12 +1005,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1025,40 +1025,40 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
@@ -1070,7 +1070,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1085,16 +1085,16 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1125,16 +1125,16 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1145,16 +1145,16 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1165,96 +1165,96 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1265,16 +1265,16 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1285,18 +1285,38 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>113</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B44" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="C43" t="n">
+      <c r="C44" t="n">
         <v>116</v>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>📅</t>
         </is>
@@ -1520,7 +1540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1579,16 +1599,16 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>18:47</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -1599,16 +1619,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1619,20 +1639,20 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -1644,7 +1664,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -1652,23 +1672,23 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -1679,16 +1699,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1699,16 +1719,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1719,16 +1739,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1739,16 +1759,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1759,16 +1779,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1779,56 +1799,56 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -1839,16 +1859,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1864,7 +1884,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -1872,43 +1892,43 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1919,20 +1939,20 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -1944,7 +1964,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -1952,23 +1972,23 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1984,7 +2004,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1999,16 +2019,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -2019,16 +2039,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -2039,16 +2059,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -2059,16 +2079,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -2084,7 +2104,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -2099,12 +2119,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -2119,40 +2139,40 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
@@ -2164,7 +2184,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -2179,16 +2199,16 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -2204,7 +2224,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -2219,16 +2239,16 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -2239,16 +2259,16 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -2259,96 +2279,96 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -2359,16 +2379,16 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -2379,18 +2399,38 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>113</v>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="B44" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="C43" t="n">
+      <c r="C44" t="n">
         <v>116</v>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>📅</t>
         </is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 30
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -505,16 +505,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -525,16 +525,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -545,20 +545,20 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -570,7 +570,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -578,23 +578,23 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -605,16 +605,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -625,16 +625,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -645,16 +645,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -665,16 +665,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -685,16 +685,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -705,56 +705,56 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -765,16 +765,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -785,36 +785,36 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -825,56 +825,56 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -885,36 +885,36 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -925,16 +925,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -945,16 +945,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -985,16 +985,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1005,16 +1005,16 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1025,12 +1025,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1045,36 +1045,36 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1085,36 +1085,36 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1125,16 +1125,16 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1145,16 +1145,16 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1165,16 +1165,16 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1185,36 +1185,36 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1225,36 +1225,36 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1265,36 +1265,36 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1305,20 +1305,120 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>108</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>111</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>112</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>113</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B48" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="C44" t="n">
+      <c r="C48" t="n">
         <v>116</v>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>116</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -1540,7 +1640,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D44"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1619,16 +1719,16 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -1639,16 +1739,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1659,20 +1759,20 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -1684,7 +1784,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -1692,23 +1792,23 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1719,16 +1819,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1739,16 +1839,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1759,16 +1859,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1779,16 +1879,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1799,16 +1899,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -1819,56 +1919,56 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1879,16 +1979,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1899,36 +1999,36 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1939,56 +2039,56 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1999,36 +2099,36 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -2039,16 +2139,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -2059,16 +2159,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -2079,16 +2179,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -2099,16 +2199,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -2119,16 +2219,16 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -2139,12 +2239,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -2159,36 +2259,36 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -2199,36 +2299,36 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -2239,16 +2339,16 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -2259,16 +2359,16 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -2279,16 +2379,16 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -2299,36 +2399,36 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -2339,36 +2439,36 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>108</v>
+        <v>81</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -2379,36 +2479,36 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -2419,20 +2519,120 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>108</v>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>111</v>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>112</v>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>113</v>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B48" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="C44" t="n">
+      <c r="C48" t="n">
         <v>116</v>
       </c>
-      <c r="D44" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>116</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>🚌</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 31
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,16 +525,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -545,16 +545,16 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -565,36 +565,36 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -605,16 +605,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -625,16 +625,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:37</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -645,7 +645,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -654,7 +654,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -665,16 +665,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -685,36 +685,36 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -725,36 +725,36 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -765,16 +765,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -785,16 +785,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -805,16 +805,16 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -825,16 +825,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -845,16 +845,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -865,16 +865,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -885,16 +885,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -905,16 +905,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -925,16 +925,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -945,16 +945,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -985,36 +985,36 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1025,16 +1025,16 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1045,16 +1045,16 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1065,36 +1065,36 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1105,16 +1105,16 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1125,16 +1125,16 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1145,16 +1145,16 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1165,16 +1165,16 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1185,16 +1185,16 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1205,16 +1205,16 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1225,16 +1225,16 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1245,56 +1245,56 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1305,47 +1305,47 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1354,7 +1354,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1365,16 +1365,16 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1385,38 +1385,418 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>70</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>70</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>80</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>80</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>80</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>81</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="C49" t="n">
+      <c r="C55" t="n">
+        <v>81</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>84</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>88</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>89</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>92</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>100</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>105</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>108</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>111</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>112</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>113</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>113</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
         <v>116</v>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>116</v>
+      </c>
+      <c r="D68" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -1433,7 +1813,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1552,36 +1932,36 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -1592,16 +1972,16 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1612,18 +1992,78 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>92</v>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>113</v>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>113</v>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="C12" t="n">
         <v>116</v>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>📅</t>
         </is>
@@ -1640,7 +2080,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1739,16 +2179,16 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -1759,16 +2199,16 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -1779,36 +2219,36 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -1819,16 +2259,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -1839,16 +2279,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:37</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -1859,7 +2299,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1868,7 +2308,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -1879,16 +2319,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -1899,36 +2339,36 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1939,36 +2379,36 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1979,16 +2419,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1999,16 +2439,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -2019,16 +2459,16 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -2039,16 +2479,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -2059,16 +2499,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -2079,16 +2519,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -2099,16 +2539,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -2119,16 +2559,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -2139,16 +2579,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -2159,16 +2599,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -2179,16 +2619,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -2199,36 +2639,36 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -2239,16 +2679,16 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -2259,16 +2699,16 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -2279,36 +2719,36 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -2319,16 +2759,16 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>69</v>
+        <v>37</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -2339,16 +2779,16 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>70</v>
+        <v>37</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -2359,16 +2799,16 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -2379,16 +2819,16 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -2399,16 +2839,16 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -2419,16 +2859,16 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>80</v>
+        <v>45</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -2439,16 +2879,16 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -2459,56 +2899,56 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>89</v>
+        <v>51</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>100</v>
+        <v>51</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -2519,47 +2959,47 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>108</v>
+        <v>51</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>111</v>
+        <v>60</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -2568,7 +3008,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>112</v>
+        <v>68</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -2579,16 +3019,16 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>113</v>
+        <v>69</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -2599,38 +3039,418 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
+          <t>19:40</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>215C_EL PATO</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>70</v>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>70</v>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>80</v>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>80</v>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>80</v>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>81</v>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>20:57</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="C49" t="n">
+      <c r="C55" t="n">
+        <v>81</v>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>84</v>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>21:04</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>88</v>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>19:59</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>89</v>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>92</v>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>100</v>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>105</v>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>108</v>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>111</v>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>112</v>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C65" t="n">
+        <v>113</v>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C66" t="n">
+        <v>113</v>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C67" t="n">
         <v>116</v>
       </c>
-      <c r="D49" t="inlineStr">
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>20:56</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>27_EL RETIRO</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>116</v>
+      </c>
+      <c r="D68" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 32
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -605,16 +605,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>19:53</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -625,7 +625,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>19:37</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -645,16 +645,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>19:37</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -665,12 +665,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>19:41</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -685,7 +685,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -694,11 +694,11 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -718,23 +718,23 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -745,16 +745,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -765,16 +765,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -785,16 +785,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -805,16 +805,16 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -825,36 +825,36 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -865,7 +865,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -874,47 +874,47 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -925,36 +925,36 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -985,36 +985,36 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1025,16 +1025,16 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1045,76 +1045,76 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1125,56 +1125,56 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1185,16 +1185,16 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1205,16 +1205,16 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1225,16 +1225,16 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1245,36 +1245,36 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1285,16 +1285,16 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1305,56 +1305,56 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1365,16 +1365,16 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1385,16 +1385,16 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1405,36 +1405,36 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1445,16 +1445,16 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1465,16 +1465,16 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1485,16 +1485,16 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1505,16 +1505,16 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1525,16 +1525,16 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1545,16 +1545,16 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1565,16 +1565,16 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1585,36 +1585,36 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1625,16 +1625,16 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -1645,36 +1645,36 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -1685,16 +1685,16 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -1705,16 +1705,16 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -1725,16 +1725,16 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -1745,16 +1745,16 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -1765,38 +1765,218 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>105</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>105</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>108</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>111</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>112</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>113</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>113</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>114</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>116</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="B77" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="C68" t="n">
+      <c r="C77" t="n">
         <v>116</v>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="D77" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -1813,7 +1993,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2052,18 +2232,38 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>114</v>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="B13" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="C13" t="n">
         <v>116</v>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>📅</t>
         </is>
@@ -2080,7 +2280,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2259,16 +2459,16 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>19:53</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -2279,7 +2479,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>19:37</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2299,16 +2499,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>19:37</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -2319,12 +2519,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>19:41</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -2339,7 +2539,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -2348,11 +2548,11 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -2364,7 +2564,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -2372,23 +2572,23 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -2399,16 +2599,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -2419,16 +2619,16 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -2439,16 +2639,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -2459,16 +2659,16 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -2479,36 +2679,36 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -2519,7 +2719,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2528,47 +2728,47 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -2579,36 +2779,36 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -2619,16 +2819,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -2639,36 +2839,36 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -2679,16 +2879,16 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -2699,76 +2899,76 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -2779,56 +2979,56 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -2839,16 +3039,16 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -2859,16 +3059,16 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -2879,16 +3079,16 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -2899,36 +3099,36 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -2939,16 +3139,16 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -2959,56 +3159,56 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -3019,16 +3219,16 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -3039,16 +3239,16 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -3059,36 +3259,36 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -3099,16 +3299,16 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -3119,16 +3319,16 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -3139,16 +3339,16 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -3159,16 +3359,16 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -3179,16 +3379,16 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -3199,16 +3399,16 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -3219,16 +3419,16 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -3239,36 +3439,36 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -3279,16 +3479,16 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -3299,36 +3499,36 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -3339,16 +3539,16 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -3359,16 +3559,16 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -3379,16 +3579,16 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -3399,16 +3599,16 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -3419,38 +3619,218 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C68" t="n">
+        <v>105</v>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="C69" t="n">
+        <v>105</v>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="C70" t="n">
+        <v>108</v>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C71" t="n">
+        <v>111</v>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C72" t="n">
+        <v>112</v>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C73" t="n">
+        <v>113</v>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C74" t="n">
+        <v>113</v>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C75" t="n">
+        <v>114</v>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C76" t="n">
+        <v>116</v>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
+      <c r="B77" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="C68" t="n">
+      <c r="C77" t="n">
         <v>116</v>
       </c>
-      <c r="D68" t="inlineStr">
+      <c r="D77" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 33
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -665,16 +665,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>20:28</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -685,16 +685,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>19:41</t>
+          <t>20:29</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -705,36 +705,36 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -745,36 +745,36 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -785,16 +785,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -805,16 +805,16 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -825,16 +825,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -845,16 +845,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -865,36 +865,36 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -905,16 +905,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -925,16 +925,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -945,36 +945,36 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -985,16 +985,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1005,16 +1005,16 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1025,56 +1025,56 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1085,16 +1085,16 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1105,16 +1105,16 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1125,36 +1125,36 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1165,16 +1165,16 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1185,7 +1185,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1194,7 +1194,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1205,16 +1205,16 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1225,56 +1225,56 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1285,16 +1285,16 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1305,36 +1305,36 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1345,16 +1345,16 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1365,16 +1365,16 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1385,16 +1385,16 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1405,16 +1405,16 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1425,16 +1425,16 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1445,16 +1445,16 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1465,16 +1465,16 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1485,16 +1485,16 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1505,36 +1505,36 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1545,16 +1545,16 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1565,16 +1565,16 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1585,16 +1585,16 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1605,16 +1605,16 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1625,16 +1625,16 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -1645,56 +1645,56 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -1705,16 +1705,16 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -1725,16 +1725,16 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -1745,16 +1745,16 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -1765,16 +1765,16 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -1785,56 +1785,56 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:53</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -1845,16 +1845,16 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -1865,16 +1865,16 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -1885,16 +1885,16 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -1905,78 +1905,318 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>101</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>104</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>105</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>105</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>108</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>111</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>112</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>113</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>113</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>114</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>114</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>116</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
+      <c r="B89" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="C77" t="n">
+      <c r="C89" t="n">
         <v>116</v>
       </c>
-      <c r="D77" t="inlineStr">
+      <c r="D89" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -1993,7 +2233,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2192,32 +2432,32 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>20:23</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -2232,38 +2472,58 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:29</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>114</v>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B14" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="C14" t="n">
         <v>116</v>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>📅</t>
         </is>
@@ -2280,7 +2540,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D77"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2519,16 +2779,16 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>20:28</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -2539,16 +2799,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>19:41</t>
+          <t>20:29</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -2559,36 +2819,36 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -2599,36 +2859,36 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -2639,16 +2899,16 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -2659,16 +2919,16 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -2679,16 +2939,16 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -2699,16 +2959,16 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -2719,36 +2979,36 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -2759,16 +3019,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -2779,16 +3039,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -2799,36 +3059,36 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -2839,16 +3099,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -2859,16 +3119,16 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -2879,56 +3139,56 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -2939,16 +3199,16 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -2959,16 +3219,16 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -2979,36 +3239,36 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -3019,16 +3279,16 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -3039,7 +3299,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3048,7 +3308,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -3059,16 +3319,16 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -3079,56 +3339,56 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -3139,16 +3399,16 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -3159,36 +3419,36 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -3199,16 +3459,16 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -3219,16 +3479,16 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -3239,16 +3499,16 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -3259,16 +3519,16 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -3279,16 +3539,16 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -3299,16 +3559,16 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -3319,16 +3579,16 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -3339,16 +3599,16 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -3359,36 +3619,36 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -3399,16 +3659,16 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -3419,16 +3679,16 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -3439,16 +3699,16 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -3459,16 +3719,16 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -3479,16 +3739,16 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -3499,56 +3759,56 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -3559,16 +3819,16 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -3579,16 +3839,16 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -3599,16 +3859,16 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -3619,16 +3879,16 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -3639,56 +3899,56 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>21:53</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -3699,16 +3959,16 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -3719,16 +3979,16 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -3739,16 +3999,16 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -3759,78 +4019,318 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="C77" t="n">
+        <v>101</v>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="C78" t="n">
+        <v>104</v>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C79" t="n">
+        <v>105</v>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="C80" t="n">
+        <v>105</v>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="C81" t="n">
+        <v>108</v>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C82" t="n">
+        <v>111</v>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C83" t="n">
+        <v>112</v>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C84" t="n">
+        <v>113</v>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C85" t="n">
+        <v>113</v>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C86" t="n">
+        <v>114</v>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C87" t="n">
+        <v>114</v>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C88" t="n">
+        <v>116</v>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="B77" t="inlineStr">
+      <c r="B89" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="C77" t="n">
+      <c r="C89" t="n">
         <v>116</v>
       </c>
-      <c r="D77" t="inlineStr">
+      <c r="D89" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 34
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -625,16 +625,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -645,7 +645,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>19:37</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -665,12 +665,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20:28</t>
+          <t>19:37</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -685,16 +685,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20:29</t>
+          <t>20:28</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -705,16 +705,16 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>20:45</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -725,16 +725,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>19:41</t>
+          <t>20:29</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -745,36 +745,36 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -785,36 +785,36 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -825,36 +825,36 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -865,7 +865,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20:47</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -874,7 +874,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -885,16 +885,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -905,16 +905,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -925,56 +925,56 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -985,16 +985,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20:53</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1005,7 +1005,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1014,27 +1014,27 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1045,16 +1045,16 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1065,16 +1065,16 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -1085,16 +1085,16 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1105,36 +1105,36 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1145,36 +1145,36 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1185,16 +1185,16 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1205,16 +1205,16 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1225,16 +1225,16 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1245,36 +1245,36 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -1285,16 +1285,16 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1305,36 +1305,36 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1345,36 +1345,36 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1385,16 +1385,16 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1405,36 +1405,36 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1445,16 +1445,16 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1465,16 +1465,16 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1485,16 +1485,16 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1505,36 +1505,36 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>21:33</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1545,16 +1545,16 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1565,36 +1565,36 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>21:32</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1605,16 +1605,16 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1625,16 +1625,16 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -1645,36 +1645,36 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -1685,16 +1685,16 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -1705,56 +1705,56 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -1765,16 +1765,16 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -1785,16 +1785,16 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>21:53</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -1805,16 +1805,16 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -1825,27 +1825,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1854,7 +1854,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -1865,36 +1865,36 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -1905,36 +1905,36 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>22:05</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -1945,36 +1945,36 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>22:04</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -1985,16 +1985,16 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -2005,76 +2005,76 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>21:53</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -2085,36 +2085,36 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -2125,16 +2125,16 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -2145,27 +2145,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>22:21</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2174,7 +2174,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2185,38 +2185,398 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
+          <t>22:05</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>98</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>100</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>101</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>101</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>22:26</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>102</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>22:27</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>103</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>104</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>105</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>105</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>108</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>111</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>112</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>113</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>113</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>114</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>114</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>22:38</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>114</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>116</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
+      <c r="B107" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="C89" t="n">
+      <c r="C107" t="n">
         <v>116</v>
       </c>
-      <c r="D89" t="inlineStr">
+      <c r="D107" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -2233,7 +2593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2292,47 +2652,47 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2341,7 +2701,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -2352,36 +2712,36 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>70</v>
+        <v>44</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -2392,87 +2752,87 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>92</v>
+        <v>62</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>22:05</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>98</v>
+        <v>70</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>22:04</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>113</v>
+        <v>80</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2481,7 +2841,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>113</v>
+        <v>84</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -2492,38 +2852,158 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>22:20</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-40 Y 115</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>96</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>22:05</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>98</v>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>113</v>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>113</v>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>114</v>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>22:38</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>114</v>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="B20" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="C20" t="n">
         <v>116</v>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>📅</t>
         </is>
@@ -2540,7 +3020,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2739,16 +3219,16 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -2759,7 +3239,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>19:37</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2779,12 +3259,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>20:28</t>
+          <t>19:37</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -2799,16 +3279,16 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>20:29</t>
+          <t>20:28</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -2819,16 +3299,16 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>20:45</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -2839,16 +3319,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>19:41</t>
+          <t>20:29</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -2859,36 +3339,36 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -2899,36 +3379,36 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -2939,36 +3419,36 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -2979,7 +3459,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>20:47</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -2988,7 +3468,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -2999,16 +3479,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -3019,16 +3499,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -3039,56 +3519,56 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -3099,16 +3579,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>20:53</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -3119,7 +3599,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -3128,27 +3608,27 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -3159,16 +3639,16 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -3179,16 +3659,16 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
@@ -3199,16 +3679,16 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -3219,36 +3699,36 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -3259,36 +3739,36 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -3299,16 +3779,16 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -3319,16 +3799,16 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -3339,16 +3819,16 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -3359,36 +3839,36 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -3399,16 +3879,16 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -3419,36 +3899,36 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -3459,36 +3939,36 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -3499,16 +3979,16 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -3519,36 +3999,36 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -3559,16 +4039,16 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -3579,16 +4059,16 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -3599,16 +4079,16 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -3619,36 +4099,36 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>21:33</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -3659,16 +4139,16 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -3679,36 +4159,36 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>21:32</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -3719,16 +4199,16 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -3739,16 +4219,16 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -3759,36 +4239,36 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>80</v>
+        <v>53</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -3799,16 +4279,16 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -3819,56 +4299,56 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -3879,16 +4359,16 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -3899,16 +4379,16 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>21:53</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -3919,16 +4399,16 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -3939,27 +4419,27 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -3968,7 +4448,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -3979,36 +4459,36 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>90</v>
+        <v>71</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -4019,36 +4499,36 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>22:05</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -4059,36 +4539,36 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>22:04</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -4099,16 +4579,16 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>104</v>
+        <v>81</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -4119,76 +4599,76 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>21:53</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -4199,36 +4679,36 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -4239,16 +4719,16 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -4259,27 +4739,27 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>22:21</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -4288,7 +4768,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -4299,38 +4779,398 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
+          <t>22:05</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C89" t="n">
+        <v>98</v>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="C90" t="n">
+        <v>100</v>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C91" t="n">
+        <v>101</v>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>22:08</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="C92" t="n">
+        <v>101</v>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>22:26</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="C93" t="n">
+        <v>102</v>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>22:27</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
+        </is>
+      </c>
+      <c r="C94" t="n">
+        <v>103</v>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>21:37</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="C95" t="n">
+        <v>104</v>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>21:21</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C96" t="n">
+        <v>105</v>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>21:38</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>17_ROMERO</t>
+        </is>
+      </c>
+      <c r="C97" t="n">
+        <v>105</v>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="C98" t="n">
+        <v>108</v>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C99" t="n">
+        <v>111</v>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C100" t="n">
+        <v>112</v>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C101" t="n">
+        <v>113</v>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C102" t="n">
+        <v>113</v>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C103" t="n">
+        <v>114</v>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C104" t="n">
+        <v>114</v>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>22:38</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C105" t="n">
+        <v>114</v>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C106" t="n">
+        <v>116</v>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
+      <c r="B107" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="C89" t="n">
+      <c r="C107" t="n">
         <v>116</v>
       </c>
-      <c r="D89" t="inlineStr">
+      <c r="D107" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 35
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -725,16 +725,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20:29</t>
+          <t>20:59</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -745,16 +745,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>20:29</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -765,12 +765,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>19:41</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -785,7 +785,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -794,11 +794,11 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -810,7 +810,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -818,63 +818,63 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -885,16 +885,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -905,16 +905,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -925,16 +925,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20:47</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -945,16 +945,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -965,16 +965,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -985,16 +985,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1005,36 +1005,36 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -1045,56 +1045,56 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20:53</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1105,36 +1105,36 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1145,36 +1145,36 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1185,7 +1185,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1194,7 +1194,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1205,16 +1205,16 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1225,36 +1225,36 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1265,36 +1265,36 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -1305,12 +1305,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -1318,23 +1318,23 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1345,16 +1345,16 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1365,16 +1365,16 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1385,12 +1385,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -1398,23 +1398,23 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -1425,16 +1425,16 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -1445,16 +1445,16 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1465,16 +1465,16 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1485,16 +1485,16 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -1505,16 +1505,16 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1525,16 +1525,16 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1545,16 +1545,16 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1565,36 +1565,36 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>21:32</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1605,36 +1605,36 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>21:32</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -1645,16 +1645,16 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -1665,16 +1665,16 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -1685,16 +1685,16 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -1705,76 +1705,76 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>21:33</t>
+          <t>21:52</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -1785,56 +1785,56 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -1845,16 +1845,16 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -1865,36 +1865,36 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -1905,16 +1905,16 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -1925,16 +1925,16 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -1945,56 +1945,56 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -2005,16 +2005,16 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -2025,16 +2025,16 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -2045,36 +2045,36 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>21:53</t>
+          <t>22:04</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -2085,36 +2085,36 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -2125,16 +2125,16 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -2145,16 +2145,16 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>22:22</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -2165,16 +2165,16 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>22:20</t>
+          <t>21:53</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2185,16 +2185,16 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>22:20</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2205,16 +2205,16 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>22:05</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -2225,16 +2225,16 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -2245,16 +2245,16 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -2265,16 +2265,16 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2285,16 +2285,16 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>22:26</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -2305,16 +2305,16 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>22:27</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -2325,96 +2325,96 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>22:39</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -2425,16 +2425,16 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>22:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -2445,16 +2445,16 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>22:27</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -2465,16 +2465,16 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -2485,16 +2485,16 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -2505,78 +2505,238 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>22:21</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>22:38</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>112</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>113</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>113</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>114</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>114</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>22:38</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>114</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>22:52</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>114</v>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>116</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="B107" t="inlineStr">
+      <c r="B115" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="C107" t="n">
+      <c r="C115" t="n">
         <v>116</v>
       </c>
-      <c r="D107" t="inlineStr">
+      <c r="D115" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -2593,7 +2753,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2912,7 +3072,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>22:39</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -2921,7 +3081,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -2932,12 +3092,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>20:23</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -2952,27 +3112,27 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:29</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>22:38</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -2985,25 +3145,45 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
+          <t>22:38</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>114</v>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="B21" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="C21" t="n">
         <v>116</v>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>📅</t>
         </is>
@@ -3020,7 +3200,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D107"/>
+  <dimension ref="A1:D115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3319,16 +3499,16 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>20:29</t>
+          <t>20:59</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -3339,16 +3519,16 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>20:29</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -3359,12 +3539,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>19:41</t>
+          <t>18:35</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -3379,7 +3559,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:41</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -3388,11 +3568,11 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -3404,7 +3584,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -3412,63 +3592,63 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>20:55</t>
+          <t>18:40</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>20:55</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>19:00</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -3479,16 +3659,16 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>18:48</t>
+          <t>19:00</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
@@ -3499,16 +3679,16 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>20:12</t>
+          <t>18:48</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -3519,16 +3699,16 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>20:47</t>
+          <t>20:12</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -3539,16 +3719,16 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>20:47</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -3559,16 +3739,16 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>18:52</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
@@ -3579,16 +3759,16 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>18:52</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -3599,36 +3779,36 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>20:01</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
@@ -3639,56 +3819,56 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>20:01</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>20:53</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -3699,36 +3879,36 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -3739,36 +3919,36 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -3779,7 +3959,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -3788,7 +3968,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -3799,16 +3979,16 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -3819,36 +3999,36 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -3859,36 +4039,36 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
@@ -3899,12 +4079,12 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -3912,23 +4092,23 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -3939,16 +4119,16 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -3959,16 +4139,16 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -3979,12 +4159,12 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -3992,23 +4172,23 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -4019,16 +4199,16 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -4039,16 +4219,16 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -4059,16 +4239,16 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -4079,16 +4259,16 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -4099,16 +4279,16 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -4119,16 +4299,16 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -4139,16 +4319,16 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -4159,36 +4339,36 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>21:32</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -4199,36 +4379,36 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>21:32</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -4239,16 +4419,16 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -4259,16 +4439,16 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -4279,16 +4459,16 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -4299,76 +4479,76 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>21:33</t>
+          <t>21:52</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -4379,56 +4559,56 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -4439,16 +4619,16 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -4459,36 +4639,36 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -4499,16 +4679,16 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -4519,16 +4699,16 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -4539,56 +4719,56 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -4599,16 +4779,16 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -4619,16 +4799,16 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -4639,36 +4819,36 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>21:53</t>
+          <t>22:04</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -4679,36 +4859,36 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -4719,16 +4899,16 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -4739,16 +4919,16 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>22:22</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -4759,16 +4939,16 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>22:20</t>
+          <t>21:53</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -4779,16 +4959,16 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>22:20</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -4799,16 +4979,16 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>22:05</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -4819,16 +4999,16 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -4839,16 +5019,16 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -4859,16 +5039,16 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -4879,16 +5059,16 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>22:26</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -4899,16 +5079,16 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>22:27</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -4919,96 +5099,96 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>22:39</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -5019,16 +5199,16 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>22:26</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -5039,16 +5219,16 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>22:27</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -5059,16 +5239,16 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -5079,16 +5259,16 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -5099,78 +5279,238 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>22:21</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>22:38</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>20:21</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C107" t="n">
+        <v>112</v>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C108" t="n">
+        <v>113</v>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C109" t="n">
+        <v>113</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C110" t="n">
+        <v>114</v>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C111" t="n">
+        <v>114</v>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>22:38</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C112" t="n">
+        <v>114</v>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>22:52</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="C113" t="n">
+        <v>114</v>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C114" t="n">
+        <v>116</v>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="B107" t="inlineStr">
+      <c r="B115" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="C107" t="n">
+      <c r="C115" t="n">
         <v>116</v>
       </c>
-      <c r="D107" t="inlineStr">
+      <c r="D115" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 36
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D115"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1085,16 +1085,16 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>22:06</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -1105,12 +1105,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20:53</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1125,16 +1125,16 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1145,52 +1145,52 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1205,7 +1205,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1214,7 +1214,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1225,7 +1225,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1234,7 +1234,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -1245,16 +1245,16 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1270,7 +1270,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -1278,43 +1278,43 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -1325,12 +1325,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -1350,7 +1350,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -1358,47 +1358,47 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -1410,7 +1410,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -1418,19 +1418,19 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -1445,16 +1445,16 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -1465,16 +1465,16 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -1490,7 +1490,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -1505,16 +1505,16 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -1525,16 +1525,16 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -1545,16 +1545,16 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>22:23</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1565,16 +1565,16 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1585,16 +1585,16 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1605,36 +1605,36 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>21:32</t>
+          <t>22:26</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -1645,16 +1645,16 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -1665,16 +1665,16 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>22:28</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -1685,16 +1685,16 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>22:28</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -1705,36 +1705,36 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:32</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -1745,36 +1745,36 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>21:52</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -1785,56 +1785,56 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>21:33</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -1845,36 +1845,36 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>21:52</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -1885,56 +1885,56 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -1945,16 +1945,16 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -1965,36 +1965,36 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -2005,16 +2005,16 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -2025,16 +2025,16 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -2045,56 +2045,56 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -2105,16 +2105,16 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -2125,16 +2125,16 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -2145,36 +2145,36 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>22:22</t>
+          <t>22:04</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>21:53</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2185,16 +2185,16 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2205,7 +2205,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>23:03</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2214,27 +2214,27 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -2245,16 +2245,16 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -2265,16 +2265,16 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>22:22</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2285,16 +2285,16 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>22:20</t>
+          <t>21:53</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -2305,16 +2305,16 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>22:20</t>
+          <t>23:08</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -2325,7 +2325,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>22:05</t>
+          <t>23:08</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2334,7 +2334,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -2345,16 +2345,16 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -2365,36 +2365,36 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -2405,16 +2405,16 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>22:39</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -2425,16 +2425,16 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>22:26</t>
+          <t>23:12</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -2445,16 +2445,16 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>22:27</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -2465,16 +2465,16 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -2485,36 +2485,36 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
@@ -2525,36 +2525,36 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -2565,16 +2565,16 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -2585,7 +2585,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>22:39</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2594,7 +2594,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
@@ -2605,16 +2605,16 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>22:26</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
@@ -2625,36 +2625,36 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>22:27</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>22:21</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -2665,56 +2665,56 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>22:38</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>22:52</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -2725,18 +2725,218 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>111</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>112</v>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>113</v>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>113</v>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>114</v>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>114</v>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>22:38</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>114</v>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>22:52</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>114</v>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>116</v>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="B115" t="inlineStr">
+      <c r="B124" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="C115" t="n">
+      <c r="C124" t="n">
         <v>116</v>
       </c>
-      <c r="D115" t="inlineStr">
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>23:39</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>118</v>
+      </c>
+      <c r="D125" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -2753,7 +2953,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2892,16 +3092,16 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>22:23</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -2912,27 +3112,27 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2941,7 +3141,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -2952,76 +3152,76 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>22:04</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
@@ -3032,56 +3232,56 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>22:20</t>
+          <t>23:08</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>22:05</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>22:39</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -3092,36 +3292,36 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>22:39</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -3132,7 +3332,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>20:23</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -3141,27 +3341,27 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>22:38</t>
+          <t>21:29</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -3172,20 +3372,80 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>114</v>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>22:38</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>114</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>20:39</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="C23" t="n">
         <v>116</v>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>23:39</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>118</v>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -3200,7 +3460,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D115"/>
+  <dimension ref="A1:D125"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3859,16 +4119,16 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>18:56</t>
+          <t>22:06</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
@@ -3879,12 +4139,12 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>20:53</t>
+          <t>18:56</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -3899,16 +4159,16 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>20:53</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -3919,52 +4179,52 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>18:58</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>18:58</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -3979,7 +4239,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>20:22</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -3988,7 +4248,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -3999,7 +4259,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>19:01</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -4008,7 +4268,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
@@ -4019,16 +4279,16 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>19:01</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -4044,7 +4304,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -4052,43 +4312,43 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>19:04</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>19:05</t>
+          <t>19:04</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -4099,12 +4359,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:05</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -4124,7 +4384,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -4132,47 +4392,47 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>21:20</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>19:20</t>
+          <t>21:20</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -4184,7 +4444,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -4192,19 +4452,19 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>20:13</t>
+          <t>19:20</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -4219,16 +4479,16 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>20:13</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
@@ -4239,16 +4499,16 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
@@ -4264,7 +4524,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -4279,16 +4539,16 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>19:12</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -4299,16 +4559,16 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
@@ -4319,16 +4579,16 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>22:23</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -4339,16 +4599,16 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -4359,16 +4619,16 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -4379,36 +4639,36 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>20:24</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>21:32</t>
+          <t>22:26</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -4419,16 +4679,16 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -4439,16 +4699,16 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>22:28</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -4459,16 +4719,16 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>19:21</t>
+          <t>22:28</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -4479,36 +4739,36 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>19:34</t>
+          <t>20:24</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>21:32</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -4519,36 +4779,36 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>21:52</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -4559,56 +4819,56 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:21</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>19:34</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>21:33</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -4619,36 +4879,36 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>20:44</t>
+          <t>21:52</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>20:52</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -4659,56 +4919,56 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>21:46</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>21:33</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -4719,16 +4979,16 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>20:44</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -4739,36 +4999,36 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -4779,16 +5039,16 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -4799,16 +5059,16 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>20:56</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -4819,56 +5079,56 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -4879,16 +5139,16 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -4899,16 +5159,16 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -4919,36 +5179,36 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>22:22</t>
+          <t>22:04</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>21:53</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -4959,16 +5219,16 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>21:04</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -4979,7 +5239,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>19:59</t>
+          <t>23:03</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -4988,27 +5248,27 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -5019,16 +5279,16 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -5039,16 +5299,16 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>22:22</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -5059,16 +5319,16 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>22:20</t>
+          <t>21:53</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -5079,16 +5339,16 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>22:20</t>
+          <t>23:08</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -5099,7 +5359,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>22:05</t>
+          <t>23:08</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -5108,7 +5368,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -5119,16 +5379,16 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>21:04</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -5139,36 +5399,36 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>19:59</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>22:08</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -5179,16 +5439,16 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>22:39</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -5199,16 +5459,16 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>22:26</t>
+          <t>23:12</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -5219,16 +5479,16 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>22:27</t>
+          <t>21:08</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -5239,16 +5499,16 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>21:37</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C102" t="n">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -5259,36 +5519,36 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>21:21</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="C103" t="n">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>21:38</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="C104" t="n">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
@@ -5299,36 +5559,36 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>20:10</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="C105" t="n">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>20:21</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>11_ETCHEVERRY</t>
         </is>
       </c>
       <c r="C106" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -5339,16 +5599,16 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>20:22</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>11_ETCHEVERRY</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C107" t="n">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -5359,7 +5619,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>20:23</t>
+          <t>22:39</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -5368,7 +5628,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
@@ -5379,16 +5639,16 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>22:26</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="C109" t="n">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D109" t="inlineStr">
         <is>
@@ -5399,36 +5659,36 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>22:27</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="C110" t="n">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="D110" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>22:21</t>
+          <t>21:37</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="C111" t="n">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D111" t="inlineStr">
         <is>
@@ -5439,56 +5699,56 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>22:38</t>
+          <t>21:21</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="C112" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D112" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>22:52</t>
+          <t>21:38</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="C113" t="n">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>20:39</t>
+          <t>20:31</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="C114" t="n">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D114" t="inlineStr">
         <is>
@@ -5499,18 +5759,218 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
+          <t>20:21</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C115" t="n">
+        <v>111</v>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>20:22</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="C116" t="n">
+        <v>112</v>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>20:23</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C117" t="n">
+        <v>113</v>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C118" t="n">
+        <v>113</v>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C119" t="n">
+        <v>114</v>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>22:21</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="C120" t="n">
+        <v>114</v>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>22:38</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>114</v>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>22:52</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>14_ABASTO</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>114</v>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>20:39</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>116</v>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="B115" t="inlineStr">
+      <c r="B124" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="C115" t="n">
+      <c r="C124" t="n">
         <v>116</v>
       </c>
-      <c r="D115" t="inlineStr">
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>23:39</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>118</v>
+      </c>
+      <c r="D125" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 38
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -469,14 +469,19 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -484,19 +489,20 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -509,29 +515,31 @@
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
+          <t>19:36</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>18:31</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>15_ABASTO</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>19:37</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -549,34 +557,30 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>19:37</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -590,7 +594,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -599,6 +603,7 @@
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
           <t>18:40</t>
@@ -619,6 +624,7 @@
       </c>
     </row>
     <row r="9">
+      <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr">
         <is>
           <t>19:51</t>
@@ -641,12 +647,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -655,7 +661,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -666,7 +672,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -680,7 +686,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -689,18 +695,23 @@
       </c>
     </row>
     <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -711,12 +722,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -725,7 +736,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -734,23 +745,19 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
+      <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -759,6 +766,7 @@
       </c>
     </row>
     <row r="15">
+      <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
           <t>20:52</t>
@@ -779,6 +787,7 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr">
         <is>
           <t>19:12</t>
@@ -799,14 +808,19 @@
       </c>
     </row>
     <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -819,6 +833,7 @@
       </c>
     </row>
     <row r="18">
+      <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr">
         <is>
           <t>19:16</t>
@@ -826,7 +841,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -834,23 +849,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="19">
+      <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -861,21 +877,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>22:20</t>
+          <t>22:22</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -884,89 +900,91 @@
       </c>
     </row>
     <row r="21">
+      <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>22:22</t>
+          <t>22:23</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="D22" t="n">
+        <v>36</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>21:22</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>38</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>22:26</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
         <v>39</v>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>22:22</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>39</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>19:10</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>16_P MOR-SANTA ANA</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>40</v>
-      </c>
       <c r="E24" t="inlineStr">
         <is>
           <t>🚌</t>
@@ -974,14 +992,19 @@
       </c>
     </row>
     <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>22:27</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -996,21 +1019,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>22:26</t>
+          <t>22:27</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1019,23 +1042,19 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
+      <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr">
         <is>
-          <t>22:27</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1044,23 +1063,19 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
+      <c r="A28" t="inlineStr"/>
       <c r="B28" t="inlineStr">
         <is>
-          <t>22:27</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1069,6 +1084,7 @@
       </c>
     </row>
     <row r="29">
+      <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr">
         <is>
           <t>21:28</t>
@@ -1089,6 +1105,7 @@
       </c>
     </row>
     <row r="30">
+      <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr">
         <is>
           <t>19:28</t>
@@ -1109,6 +1126,7 @@
       </c>
     </row>
     <row r="31">
+      <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
           <t>19:17</t>
@@ -1131,12 +1149,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>22:38</t>
+          <t>22:39</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -1145,7 +1163,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1154,6 +1172,7 @@
       </c>
     </row>
     <row r="33">
+      <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr">
         <is>
           <t>19:30</t>
@@ -1176,7 +1195,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1190,7 +1209,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1199,6 +1218,7 @@
       </c>
     </row>
     <row r="35">
+      <c r="A35" t="inlineStr"/>
       <c r="B35" t="inlineStr">
         <is>
           <t>20:09</t>
@@ -1219,6 +1239,7 @@
       </c>
     </row>
     <row r="36">
+      <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
           <t>19:40</t>
@@ -1241,12 +1262,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>23:03</t>
+          <t>23:04</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -1255,7 +1276,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1264,14 +1285,19 @@
       </c>
     </row>
     <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>23:07</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -1284,6 +1310,7 @@
       </c>
     </row>
     <row r="39">
+      <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr">
         <is>
           <t>19:50</t>
@@ -1291,7 +1318,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1304,18 +1331,19 @@
       </c>
     </row>
     <row r="40">
+      <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1324,14 +1352,19 @@
       </c>
     </row>
     <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>23:08</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1344,23 +1377,19 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
+      <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
-          <t>23:07</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1369,31 +1398,28 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
+      <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
-          <t>23:07</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="44">
+      <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr">
         <is>
           <t>19:54</t>
@@ -1416,12 +1442,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>23:11</t>
+          <t>23:13</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -1430,7 +1456,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1439,6 +1465,7 @@
       </c>
     </row>
     <row r="46">
+      <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr">
         <is>
           <t>21:23</t>
@@ -1459,6 +1486,7 @@
       </c>
     </row>
     <row r="47">
+      <c r="A47" t="inlineStr"/>
       <c r="B47" t="inlineStr">
         <is>
           <t>21:08</t>
@@ -1479,6 +1507,7 @@
       </c>
     </row>
     <row r="48">
+      <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr">
         <is>
           <t>20:10</t>
@@ -1499,6 +1528,7 @@
       </c>
     </row>
     <row r="49">
+      <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr">
         <is>
           <t>20:31</t>
@@ -1519,14 +1549,19 @@
       </c>
     </row>
     <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>23:40</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1539,43 +1574,40 @@
       </c>
     </row>
     <row r="51">
+      <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr">
         <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>113</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D51" t="n">
+      <c r="D52" t="n">
         <v>116</v>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>23:40</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D52" t="n">
-        <v>117</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1639,12 +1671,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1653,7 +1685,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -1664,12 +1696,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -1678,7 +1710,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -1687,6 +1719,7 @@
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
           <t>21:07</t>
@@ -1707,6 +1740,7 @@
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
           <t>19:12</t>
@@ -1729,12 +1763,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>22:22</t>
+          <t>22:23</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1743,7 +1777,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -1752,6 +1786,7 @@
       </c>
     </row>
     <row r="7">
+      <c r="A7" t="inlineStr"/>
       <c r="B7" t="inlineStr">
         <is>
           <t>19:10</t>
@@ -1772,6 +1807,7 @@
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
           <t>21:28</t>
@@ -1794,12 +1830,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>22:38</t>
+          <t>22:39</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1808,7 +1844,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -1817,6 +1853,7 @@
       </c>
     </row>
     <row r="10">
+      <c r="A10" t="inlineStr"/>
       <c r="B10" t="inlineStr">
         <is>
           <t>19:40</t>
@@ -1839,12 +1876,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>23:07</t>
+          <t>23:08</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1853,15 +1890,16 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="12">
+      <c r="A12" t="inlineStr"/>
       <c r="B12" t="inlineStr">
         <is>
           <t>19:54</t>
@@ -1882,6 +1920,7 @@
       </c>
     </row>
     <row r="13">
+      <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr">
         <is>
           <t>21:08</t>
@@ -1902,14 +1941,19 @@
       </c>
     </row>
     <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>23:40</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D14" t="n">
@@ -1922,23 +1966,19 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
+      <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>23:40</t>
+          <t>21:29</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -2000,14 +2040,19 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -2015,19 +2060,20 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>18:30</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -2040,29 +2086,31 @@
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
+          <t>19:36</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>18:31</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>15_ABASTO</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>19:37</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2080,34 +2128,30 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
+      <c r="A6" t="inlineStr"/>
       <c r="B6" t="inlineStr">
         <is>
-          <t>21:46</t>
+          <t>19:37</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2121,7 +2165,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -2130,6 +2174,7 @@
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
           <t>18:40</t>
@@ -2150,6 +2195,7 @@
       </c>
     </row>
     <row r="9">
+      <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr">
         <is>
           <t>19:51</t>
@@ -2172,12 +2218,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>22:04</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -2186,7 +2232,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -2197,7 +2243,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2211,7 +2257,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -2220,18 +2266,23 @@
       </c>
     </row>
     <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21:07</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -2242,12 +2293,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -2256,7 +2307,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -2265,23 +2316,19 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
+      <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr">
         <is>
-          <t>22:07</t>
+          <t>21:07</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>215B_EL PATO</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2290,6 +2337,7 @@
       </c>
     </row>
     <row r="15">
+      <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
           <t>20:52</t>
@@ -2310,6 +2358,7 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" t="inlineStr"/>
       <c r="B16" t="inlineStr">
         <is>
           <t>19:12</t>
@@ -2330,14 +2379,19 @@
       </c>
     </row>
     <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>22:20</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -2350,6 +2404,7 @@
       </c>
     </row>
     <row r="18">
+      <c r="A18" t="inlineStr"/>
       <c r="B18" t="inlineStr">
         <is>
           <t>19:16</t>
@@ -2357,7 +2412,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -2365,23 +2420,24 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="19">
+      <c r="A19" t="inlineStr"/>
       <c r="B19" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>19:16</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -2392,21 +2448,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>22:20</t>
+          <t>22:22</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>26_HERNANDEZ</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -2415,89 +2471,91 @@
       </c>
     </row>
     <row r="21">
+      <c r="A21" t="inlineStr"/>
       <c r="B21" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>22:22</t>
+          <t>22:23</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="D22" t="n">
+        <v>36</v>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>21:22</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>38</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>22:26</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
         <v>39</v>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>22:22</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>39</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>19:10</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>16_P MOR-SANTA ANA</t>
-        </is>
-      </c>
-      <c r="D24" t="n">
-        <v>40</v>
-      </c>
       <c r="E24" t="inlineStr">
         <is>
           <t>🚌</t>
@@ -2505,14 +2563,19 @@
       </c>
     </row>
     <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>22:27</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>10_OLMOS</t>
         </is>
       </c>
       <c r="D25" t="n">
@@ -2527,21 +2590,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>22:26</t>
+          <t>22:27</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -2550,23 +2613,19 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
+      <c r="A27" t="inlineStr"/>
       <c r="B27" t="inlineStr">
         <is>
-          <t>22:27</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>10_OLMOS</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -2575,23 +2634,19 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
+      <c r="A28" t="inlineStr"/>
       <c r="B28" t="inlineStr">
         <is>
-          <t>22:27</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -2600,6 +2655,7 @@
       </c>
     </row>
     <row r="29">
+      <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr">
         <is>
           <t>21:28</t>
@@ -2620,6 +2676,7 @@
       </c>
     </row>
     <row r="30">
+      <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr">
         <is>
           <t>19:28</t>
@@ -2640,6 +2697,7 @@
       </c>
     </row>
     <row r="31">
+      <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
           <t>19:17</t>
@@ -2662,12 +2720,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>22:38</t>
+          <t>22:39</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2676,7 +2734,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -2685,6 +2743,7 @@
       </c>
     </row>
     <row r="33">
+      <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr">
         <is>
           <t>19:30</t>
@@ -2707,7 +2766,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -2721,7 +2780,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2730,6 +2789,7 @@
       </c>
     </row>
     <row r="35">
+      <c r="A35" t="inlineStr"/>
       <c r="B35" t="inlineStr">
         <is>
           <t>20:09</t>
@@ -2750,6 +2810,7 @@
       </c>
     </row>
     <row r="36">
+      <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
           <t>19:40</t>
@@ -2772,12 +2833,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>23:03</t>
+          <t>23:04</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -2786,7 +2847,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -2795,14 +2856,19 @@
       </c>
     </row>
     <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>23:07</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D38" t="n">
@@ -2815,6 +2881,7 @@
       </c>
     </row>
     <row r="39">
+      <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr">
         <is>
           <t>19:50</t>
@@ -2822,7 +2889,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -2835,18 +2902,19 @@
       </c>
     </row>
     <row r="40">
+      <c r="A40" t="inlineStr"/>
       <c r="B40" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>19:50</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2855,14 +2923,19 @@
       </c>
     </row>
     <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>23:08</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -2875,23 +2948,19 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
+      <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
-          <t>23:07</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -2900,31 +2969,28 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
+      <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
-          <t>23:07</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="44">
+      <c r="A44" t="inlineStr"/>
       <c r="B44" t="inlineStr">
         <is>
           <t>19:54</t>
@@ -2947,12 +3013,12 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>21:43</t>
+          <t>21:47</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>23:11</t>
+          <t>23:13</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -2961,7 +3027,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -2970,6 +3036,7 @@
       </c>
     </row>
     <row r="46">
+      <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr">
         <is>
           <t>21:23</t>
@@ -2990,6 +3057,7 @@
       </c>
     </row>
     <row r="47">
+      <c r="A47" t="inlineStr"/>
       <c r="B47" t="inlineStr">
         <is>
           <t>21:08</t>
@@ -3010,6 +3078,7 @@
       </c>
     </row>
     <row r="48">
+      <c r="A48" t="inlineStr"/>
       <c r="B48" t="inlineStr">
         <is>
           <t>20:10</t>
@@ -3030,6 +3099,7 @@
       </c>
     </row>
     <row r="49">
+      <c r="A49" t="inlineStr"/>
       <c r="B49" t="inlineStr">
         <is>
           <t>20:31</t>
@@ -3050,14 +3120,19 @@
       </c>
     </row>
     <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>23:40</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -3070,43 +3145,40 @@
       </c>
     </row>
     <row r="51">
+      <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr">
         <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>113</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C52" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D51" t="n">
+      <c r="D52" t="n">
         <v>116</v>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>21:43</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>23:40</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D52" t="n">
-        <v>117</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 39
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,12 +497,12 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -518,16 +518,16 @@
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -539,7 +539,7 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>19:37</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -557,44 +557,44 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>19:37</t>
+          <t>21:52</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>18:40</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>21:52</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>10_OLMOS</t>
-        </is>
-      </c>
       <c r="D7" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -606,16 +606,16 @@
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -624,23 +624,27 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
@@ -652,20 +656,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>22:05</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -677,91 +681,87 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>22:06</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>21</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>23</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>25</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>23:18</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>23:46</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>16_SANTA ANA</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>19</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>22:07</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>17_ROMERO</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>20</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>22:08</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>11_ETCHEVERRY</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>21</v>
-      </c>
-      <c r="E13" t="inlineStr">
+      <c r="D14" t="n">
+        <v>28</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>📅</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>21:07</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>23</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -769,58 +769,58 @@
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>29</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>22:20</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>33</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>19:16</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>15_ABASTO</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>25</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>📅</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>19:12</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>29</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>22:20</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -841,7 +841,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -849,45 +849,45 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>22:22</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
+      <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr">
         <is>
-          <t>22:22</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -895,49 +895,49 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>22:23</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
+      <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr">
         <is>
-          <t>22:23</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -946,19 +946,23 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>23:18</t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>23:58</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -969,21 +973,21 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>23:18</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>22:26</t>
+          <t>23:58</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1318,7 +1322,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -1331,19 +1335,23 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr"/>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>23:08</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1352,19 +1360,15 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
+      <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr">
         <is>
-          <t>23:08</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -1380,12 +1384,12 @@
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -1401,16 +1405,16 @@
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1419,19 +1423,23 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr"/>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>23:13</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1440,23 +1448,19 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
+      <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr">
         <is>
-          <t>23:13</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1465,19 +1469,23 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr"/>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>23:18</t>
+        </is>
+      </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>00:49</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1549,19 +1557,15 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
+      <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr">
         <is>
-          <t>23:40</t>
+          <t>21:29</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -1577,39 +1581,18 @@
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E51" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr"/>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>20:56</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>27_EL RETIRO</t>
-        </is>
-      </c>
-      <c r="D52" t="n">
-        <v>116</v>
-      </c>
-      <c r="E52" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -1786,15 +1769,19 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>23:18</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>23:58</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -1810,108 +1797,108 @@
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
+          <t>19:10</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>40</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="inlineStr">
+        <is>
           <t>21:28</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="D9" t="n">
         <v>44</v>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>22:39</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>52</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr">
         <is>
           <t>19:40</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D11" t="n">
         <v>70</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>23:08</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D12" t="n">
         <v>81</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>19:54</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>84</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -1923,41 +1910,37 @@
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="inlineStr">
         <is>
+          <t>19:54</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>84</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="inlineStr">
+        <is>
           <t>21:08</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>215B_EL PATO</t>
         </is>
       </c>
-      <c r="D13" t="n">
+      <c r="D14" t="n">
         <v>92</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>23:40</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>113</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1997,7 +1980,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2068,12 +2051,12 @@
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="inlineStr">
         <is>
-          <t>18:30</t>
+          <t>19:36</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -2089,16 +2072,16 @@
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="inlineStr">
         <is>
-          <t>19:36</t>
+          <t>18:31</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -2110,7 +2093,7 @@
       <c r="A5" t="inlineStr"/>
       <c r="B5" t="inlineStr">
         <is>
-          <t>18:31</t>
+          <t>19:37</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -2128,44 +2111,44 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>19:37</t>
+          <t>21:52</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>10_OLMOS</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>18:40</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>21:52</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>10_OLMOS</t>
-        </is>
-      </c>
       <c r="D7" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -2177,16 +2160,16 @@
       <c r="A8" t="inlineStr"/>
       <c r="B8" t="inlineStr">
         <is>
-          <t>18:40</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -2195,23 +2178,27 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>22:05</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
@@ -2223,20 +2210,20 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>22:05</t>
+          <t>22:07</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -2248,91 +2235,87 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>22:06</t>
+          <t>22:08</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>11_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>21</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>21:07</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>23</v>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>20:52</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>25</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>23:18</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>23:46</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>16_SANTA ANA</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>19</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>22:07</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>17_ROMERO</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>20</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>22:08</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>11_ETCHEVERRY</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>21</v>
-      </c>
-      <c r="E13" t="inlineStr">
+      <c r="D14" t="n">
+        <v>28</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>📅</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>21:07</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>215B_EL PATO</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>23</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -2340,58 +2323,58 @@
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
-          <t>20:52</t>
+          <t>19:12</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>29</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>22:20</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>26_HERNANDEZ</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>33</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>19:16</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>15_ABASTO</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>25</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>📅</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>19:12</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>29</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>22:20</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>26_HERNANDEZ</t>
         </is>
       </c>
       <c r="D17" t="n">
@@ -2412,7 +2395,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D18" t="n">
@@ -2420,45 +2403,45 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>19:16</t>
+          <t>22:22</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
+      <c r="A20" t="inlineStr"/>
       <c r="B20" t="inlineStr">
         <is>
-          <t>22:22</t>
+          <t>20:11</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>16_P MOR-167 Y 521</t>
         </is>
       </c>
       <c r="D20" t="n">
@@ -2466,49 +2449,49 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>20:11</t>
+          <t>22:23</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>215B_LP-P MOR-40 Y 115</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
+      <c r="A22" t="inlineStr"/>
       <c r="B22" t="inlineStr">
         <is>
-          <t>22:23</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-40 Y 115</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -2517,19 +2500,23 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>23:18</t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>23:58</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -2540,21 +2527,21 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>23:18</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>22:26</t>
+          <t>23:58</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -2889,7 +2876,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D39" t="n">
@@ -2902,19 +2889,23 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr"/>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>23:08</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215A_LA PLATA</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2923,19 +2914,15 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
+      <c r="A41" t="inlineStr"/>
       <c r="B41" t="inlineStr">
         <is>
-          <t>23:08</t>
+          <t>19:51</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>81_EL PELIGRO</t>
         </is>
       </c>
       <c r="D41" t="n">
@@ -2951,12 +2938,12 @@
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>20:57</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D42" t="n">
@@ -2972,16 +2959,16 @@
       <c r="A43" t="inlineStr"/>
       <c r="B43" t="inlineStr">
         <is>
-          <t>20:57</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -2990,19 +2977,23 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr"/>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>19:54</t>
+          <t>23:13</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -3011,23 +3002,19 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
+      <c r="A45" t="inlineStr"/>
       <c r="B45" t="inlineStr">
         <is>
-          <t>23:13</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>23_HERNANDEZ</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -3036,19 +3023,23 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr"/>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>23:18</t>
+        </is>
+      </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>00:49</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -3120,19 +3111,15 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
+      <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr">
         <is>
-          <t>23:40</t>
+          <t>21:29</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D50" t="n">
@@ -3148,39 +3135,18 @@
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>20:56</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="E51" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr"/>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>20:56</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>27_EL RETIRO</t>
-        </is>
-      </c>
-      <c r="D52" t="n">
-        <v>116</v>
-      </c>
-      <c r="E52" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 40
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -743,7 +743,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>23:18</t>
+          <t>23:20</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -757,7 +757,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -925,15 +925,19 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>23:20</t>
+        </is>
+      </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>23:58</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -948,7 +952,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>23:18</t>
+          <t>23:20</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -958,11 +962,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -971,23 +975,19 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>23:18</t>
-        </is>
-      </c>
+      <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr">
         <is>
-          <t>23:58</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1448,44 +1448,44 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr"/>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>23:20</t>
+        </is>
+      </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>00:49</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>89</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr">
+        <is>
           <t>21:23</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D45" t="n">
+      <c r="D46" t="n">
         <v>90</v>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>23:18</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>00:49</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>16_SANTA ANA</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
-        <v>91</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1771,7 +1771,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>23:18</t>
+          <t>23:20</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1785,7 +1785,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -2297,7 +2297,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>23:18</t>
+          <t>23:20</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -2311,7 +2311,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -2479,15 +2479,19 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>23:20</t>
+        </is>
+      </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>21:22</t>
+          <t>23:58</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D22" t="n">
@@ -2502,7 +2506,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>23:18</t>
+          <t>23:20</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -2512,11 +2516,11 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>11X44_ETCHEVERRY</t>
+          <t>215_ALUAR</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -2525,23 +2529,19 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>23:18</t>
-        </is>
-      </c>
+      <c r="A24" t="inlineStr"/>
       <c r="B24" t="inlineStr">
         <is>
-          <t>23:58</t>
+          <t>21:22</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>215_ALUAR</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -3002,44 +3002,44 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr"/>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>23:20</t>
+        </is>
+      </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>00:49</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
+        <v>89</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr"/>
+      <c r="B46" t="inlineStr">
+        <is>
           <t>21:23</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>15_ABASTO</t>
         </is>
       </c>
-      <c r="D45" t="n">
+      <c r="D46" t="n">
         <v>90</v>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>23:18</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>00:49</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>16_SANTA ANA</t>
-        </is>
-      </c>
-      <c r="D46" t="n">
-        <v>91</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
📊 Arribos 141 actualizados - 41
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -927,12 +927,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>23:20</t>
+          <t>23:22</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>23:58</t>
+          <t>23:59</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -941,7 +941,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -952,38 +952,42 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>23:22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>23:59</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>37</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>23:20</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>23:58</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>38</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>21:22</t>
-        </is>
-      </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -998,63 +1002,63 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>23:20</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>23:58</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>38</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>21:22</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>38</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>22:27</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>40</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>22:27</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>40</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr"/>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>19:10</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -1067,15 +1071,19 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>22:27</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -1091,16 +1099,16 @@
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1112,16 +1120,16 @@
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1133,16 +1141,16 @@
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1151,23 +1159,19 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
+      <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr">
         <is>
-          <t>22:39</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1179,41 +1183,41 @@
       <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>23:22</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>22:51</t>
+          <t>00:11</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1222,19 +1226,23 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr"/>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>22:39</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1246,20 +1254,20 @@
       <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
@@ -1271,16 +1279,16 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>23:04</t>
+          <t>22:51</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1289,23 +1297,19 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
+      <c r="A38" t="inlineStr"/>
       <c r="B38" t="inlineStr">
         <is>
-          <t>23:07</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1317,16 +1321,16 @@
       <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1342,16 +1346,16 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>23:08</t>
+          <t>23:04</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1360,19 +1364,23 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr"/>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>23:07</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1384,87 +1392,83 @@
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>80</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>23:08</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>81</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>81</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>20:57</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D42" t="n">
+      <c r="D45" t="n">
         <v>81</v>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr"/>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>19:54</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>84</v>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>23:13</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>23_HERNANDEZ</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
-        <v>86</v>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>23:20</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>00:49</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>16_SANTA ANA</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>89</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1476,16 +1480,16 @@
       <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1494,19 +1498,23 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr"/>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>23:13</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1515,19 +1523,23 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr"/>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>23:22</t>
+        </is>
+      </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>00:50</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1536,23 +1548,27 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr"/>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>23:20</t>
+        </is>
+      </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>00:49</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -1560,16 +1576,16 @@
       <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1581,18 +1597,102 @@
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr">
         <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>92</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>100</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>108</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>113</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C55" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D51" t="n">
+      <c r="D55" t="n">
         <v>116</v>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -1609,7 +1709,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1771,42 +1871,46 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>23:22</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>23:59</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>37</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
           <t>23:20</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B8" t="inlineStr">
         <is>
           <t>23:58</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>215_ALUAR</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="D8" t="n">
         <v>38</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>19:10</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>40</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -1818,108 +1922,108 @@
       <c r="A9" t="inlineStr"/>
       <c r="B9" t="inlineStr">
         <is>
+          <t>19:10</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>215B_LP-P MOR-1 Y 57</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>40</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="inlineStr">
+        <is>
           <t>21:28</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>44</v>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>22:39</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="D11" t="n">
         <v>52</v>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr">
         <is>
           <t>19:40</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>215C_EL PATO</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="D12" t="n">
         <v>70</v>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>23:08</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>215A_LA PLATA</t>
         </is>
       </c>
-      <c r="D12" t="n">
+      <c r="D13" t="n">
         <v>81</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>19:54</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D13" t="n">
-        <v>84</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -1931,16 +2035,16 @@
       <c r="A14" t="inlineStr"/>
       <c r="B14" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -1952,18 +2056,39 @@
       <c r="A15" t="inlineStr"/>
       <c r="B15" t="inlineStr">
         <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>92</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>21:29</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>215C_LA PLATA</t>
         </is>
       </c>
-      <c r="D15" t="n">
+      <c r="D16" t="n">
         <v>113</v>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -1980,7 +2105,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2481,12 +2606,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>23:20</t>
+          <t>23:22</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>23:58</t>
+          <t>23:59</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2495,7 +2620,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -2506,38 +2631,42 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
+          <t>23:22</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>23:59</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>37</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
           <t>23:20</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="B24" t="inlineStr">
         <is>
           <t>23:58</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="D23" t="n">
-        <v>38</v>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr"/>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>21:22</t>
-        </is>
-      </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>11X44_ETCHEVERRY</t>
         </is>
       </c>
       <c r="D24" t="n">
@@ -2552,63 +2681,63 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>23:20</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>23:58</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>38</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>21:22</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>15_ABASTO</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>38</v>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
           <t>22:27</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t>10_OLMOS</t>
-        </is>
-      </c>
-      <c r="D25" t="n">
-        <v>40</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>22:27</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>84_COLONIA URQUIZA-ESC 49</t>
-        </is>
-      </c>
-      <c r="D26" t="n">
-        <v>40</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr"/>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>19:10</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D27" t="n">
@@ -2621,15 +2750,19 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>19:10</t>
+          <t>22:27</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>215B_LP-P MOR-1 Y 57</t>
+          <t>84_COLONIA URQUIZA-ESC 49</t>
         </is>
       </c>
       <c r="D28" t="n">
@@ -2645,16 +2778,16 @@
       <c r="A29" t="inlineStr"/>
       <c r="B29" t="inlineStr">
         <is>
-          <t>21:28</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>16_P MOR-SANTA ANA</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -2666,16 +2799,16 @@
       <c r="A30" t="inlineStr"/>
       <c r="B30" t="inlineStr">
         <is>
-          <t>19:28</t>
+          <t>19:10</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215B_LP-P MOR-1 Y 57</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -2687,16 +2820,16 @@
       <c r="A31" t="inlineStr"/>
       <c r="B31" t="inlineStr">
         <is>
-          <t>19:17</t>
+          <t>21:28</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>27_EL RETIRO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -2705,23 +2838,19 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
+      <c r="A32" t="inlineStr"/>
       <c r="B32" t="inlineStr">
         <is>
-          <t>22:39</t>
+          <t>19:28</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>215A_EL PATO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -2733,41 +2862,41 @@
       <c r="A33" t="inlineStr"/>
       <c r="B33" t="inlineStr">
         <is>
-          <t>19:30</t>
+          <t>19:17</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>27_EL RETIRO</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>21:47</t>
+          <t>23:22</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>22:51</t>
+          <t>00:11</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>14_ABASTO</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2776,19 +2905,23 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr"/>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>20:09</t>
+          <t>22:39</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215A_EL PATO</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -2800,20 +2933,20 @@
       <c r="A36" t="inlineStr"/>
       <c r="B36" t="inlineStr">
         <is>
-          <t>19:40</t>
+          <t>19:30</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>215C_EL PATO</t>
+          <t>225_GOMEZ</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>🚌</t>
+          <t>📅</t>
         </is>
       </c>
     </row>
@@ -2825,16 +2958,16 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>23:04</t>
+          <t>22:51</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>17_ROMERO</t>
+          <t>14_ABASTO</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -2843,23 +2976,19 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
+      <c r="A38" t="inlineStr"/>
       <c r="B38" t="inlineStr">
         <is>
-          <t>23:07</t>
+          <t>20:09</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>14X44_ABASTO</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D38" t="n">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -2871,16 +3000,16 @@
       <c r="A39" t="inlineStr"/>
       <c r="B39" t="inlineStr">
         <is>
-          <t>19:50</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>16_P MOR-SANTA ANA</t>
+          <t>215C_EL PATO</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -2896,16 +3025,16 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>23:08</t>
+          <t>23:04</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>215A_LA PLATA</t>
+          <t>17_ROMERO</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -2914,19 +3043,23 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr"/>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>19:51</t>
+          <t>23:07</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>81_EL PELIGRO</t>
+          <t>14X44_ABASTO</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -2938,87 +3071,83 @@
       <c r="A42" t="inlineStr"/>
       <c r="B42" t="inlineStr">
         <is>
+          <t>19:50</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>16_P MOR-SANTA ANA</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>80</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>23:08</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>215A_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>81</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>19:51</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>81_EL PELIGRO</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>81</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr"/>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>20:57</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D42" t="n">
+      <c r="D45" t="n">
         <v>81</v>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr"/>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>19:54</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>215C_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D43" t="n">
-        <v>84</v>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>23:13</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>23_HERNANDEZ</t>
-        </is>
-      </c>
-      <c r="D44" t="n">
-        <v>86</v>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>23:20</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>00:49</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>16_SANTA ANA</t>
-        </is>
-      </c>
-      <c r="D45" t="n">
-        <v>89</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -3030,16 +3159,16 @@
       <c r="A46" t="inlineStr"/>
       <c r="B46" t="inlineStr">
         <is>
-          <t>21:23</t>
+          <t>19:54</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>15_ABASTO</t>
+          <t>215C_LA PLATA</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -3048,19 +3177,23 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr"/>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>21:08</t>
+          <t>23:13</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>215B_EL PATO</t>
+          <t>23_HERNANDEZ</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -3069,19 +3202,23 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr"/>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>23:22</t>
+        </is>
+      </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>20:10</t>
+          <t>00:50</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>16_P MOR-167 Y 521</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -3090,23 +3227,27 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr"/>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>23:20</t>
+        </is>
+      </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>20:31</t>
+          <t>00:49</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>225_GOMEZ</t>
+          <t>16_SANTA ANA</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>📅</t>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -3114,16 +3255,16 @@
       <c r="A50" t="inlineStr"/>
       <c r="B50" t="inlineStr">
         <is>
-          <t>21:29</t>
+          <t>21:23</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>215C_LA PLATA</t>
+          <t>15_ABASTO</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>113</v>
+        <v>90</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -3135,18 +3276,102 @@
       <c r="A51" t="inlineStr"/>
       <c r="B51" t="inlineStr">
         <is>
+          <t>21:08</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>215B_EL PATO</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>92</v>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr"/>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>20:10</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>16_P MOR-167 Y 521</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>100</v>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr"/>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>20:31</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>225_GOMEZ</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>108</v>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr"/>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>21:29</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>215C_LA PLATA</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>113</v>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr"/>
+      <c r="B55" t="inlineStr">
+        <is>
           <t>20:56</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="C55" t="inlineStr">
         <is>
           <t>27_EL RETIRO</t>
         </is>
       </c>
-      <c r="D51" t="n">
+      <c r="D55" t="n">
         <v>116</v>
       </c>
-      <c r="E51" t="inlineStr">
+      <c r="E55" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>

</xml_diff>

<commit_message>
📊 Horarios actualizados Línea 141 - 44
</commit_message>
<xml_diff>
--- a/data/horarios-141-2026-01-09.xlsx
+++ b/data/horarios-141-2026-01-09.xlsx
@@ -57,9 +57,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -428,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,54 +441,109 @@
           <t>LÍNEA 141 - TODOS - 09/01/2026 23:34:00</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 5</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 7</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 8</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 9</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Bandera</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>21:47.1</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>23:36:52</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>23:46</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>10</v>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t>📅</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>Bandera</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>Estado</t>
         </is>
       </c>
     </row>
@@ -499,27 +553,32 @@
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>23:34:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>23:46</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>16_SANTA ANA</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>12</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>📅</t>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>23:36:52</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>23:52</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>16</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -529,25 +588,30 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>23:34:00</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>23:56</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>23:36:52</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>23:58</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
         <v>22</v>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -559,85 +623,89 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>23:34:00</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>23:59</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>11X44_ETCHEVERRY</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>25</v>
-      </c>
-      <c r="J5" t="inlineStr">
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>23:36:52</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>00:47</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>71</v>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>21:47.1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>23:34:00</t>
+          <t>Hora_Scrap</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>00:49</t>
+          <t>Hora_Llegada</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>75</v>
+          <t>Bandera</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>19:36</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>16_P MOR-SANTA ANA</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -650,7 +718,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -664,116 +732,166 @@
           <t>LÍNEA 141 - 215 - 09/01/2026 23:34:00</t>
         </is>
       </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 5</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 7</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 8</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 9</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Bandera</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>23:36:52</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>23:52</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>16</v>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>🚌</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
         <is>
           <t>21:47</t>
         </is>
       </c>
-      <c r="B2" s="2" t="inlineStr">
+      <c r="B3" t="inlineStr">
         <is>
           <t>21:47.1</t>
         </is>
       </c>
-      <c r="C2" s="2" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>215A_EL PATO</t>
         </is>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>📅</t>
         </is>
       </c>
-      <c r="F2" s="2" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>Hora_Scrap</t>
         </is>
       </c>
-      <c r="G2" s="2" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Hora_Llegada</t>
         </is>
       </c>
-      <c r="H2" s="2" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Bandera</t>
         </is>
       </c>
-      <c r="I2" s="2" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Minutos</t>
         </is>
       </c>
-      <c r="J2" s="2" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>Estado</t>
         </is>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr"/>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>23:34:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>23:56</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>22</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>22:05</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>215A_LA PLATA</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>18</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>📅</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -786,7 +904,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -797,57 +915,112 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>LÍNEA 141 - COMBINADAS - 09/01/2026 23:34:00</t>
+          <t>LÍNEA 141 - TODOS - 09/01/2026 23:34:00</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 5</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 6</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 7</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 8</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 9</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Hora_Scrap</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Hora_Llegada</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Bandera</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Estado</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t>21:47</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="inlineStr">
-        <is>
-          <t>21:47.1</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="inlineStr">
-        <is>
-          <t>215A_EL PATO</t>
-        </is>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="2" t="inlineStr">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>23:36:52</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>23:46</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="N2" t="n">
+        <v>10</v>
+      </c>
+      <c r="O2" t="inlineStr">
         <is>
           <t>📅</t>
-        </is>
-      </c>
-      <c r="F2" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Scrap</t>
-        </is>
-      </c>
-      <c r="G2" s="2" t="inlineStr">
-        <is>
-          <t>Hora_Llegada</t>
-        </is>
-      </c>
-      <c r="H2" s="2" t="inlineStr">
-        <is>
-          <t>Bandera</t>
-        </is>
-      </c>
-      <c r="I2" s="2" t="inlineStr">
-        <is>
-          <t>Minutos</t>
-        </is>
-      </c>
-      <c r="J2" s="2" t="inlineStr">
-        <is>
-          <t>Estado</t>
         </is>
       </c>
     </row>
@@ -857,27 +1030,32 @@
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>23:34:00</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>23:46</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>16_SANTA ANA</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>12</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>📅</t>
+      <c r="F3" t="inlineStr"/>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>23:36:52</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>23:52</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>215_ALUAR</t>
+        </is>
+      </c>
+      <c r="N3" t="n">
+        <v>16</v>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>🚌</t>
         </is>
       </c>
     </row>
@@ -887,25 +1065,30 @@
       <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>23:34:00</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>23:56</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>215_ALUAR</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>23:36:52</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>23:58</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>11X44_ETCHEVERRY</t>
+        </is>
+      </c>
+      <c r="N4" t="n">
         <v>22</v>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
@@ -917,85 +1100,89 @@
       <c r="C5" t="inlineStr"/>
       <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>23:34:00</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>23:59</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>11X44_ETCHEVERRY</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>25</v>
-      </c>
-      <c r="J5" t="inlineStr">
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>23:36:52</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>00:47</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>16_SANTA ANA</t>
+        </is>
+      </c>
+      <c r="N5" t="n">
+        <v>71</v>
+      </c>
+      <c r="O5" t="inlineStr">
         <is>
           <t>🚌</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>21:47</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>21:47.1</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>215A_EL PATO</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>📅</t>
+        </is>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>23:34:00</t>
+          <t>Hora_Scrap</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>00:49</t>
+          <t>Hora_Llegada</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>16_SANTA ANA</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>75</v>
+          <t>Bandera</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Minutos</t>
+        </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>🚌</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr"/>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>19:36</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>16_P MOR-SANTA ANA</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>🚌</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>